<commit_message>
good version of project
</commit_message>
<xml_diff>
--- a/TraceChart.xlsx
+++ b/TraceChart.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="243">
   <si>
     <t>Byte value</t>
   </si>
@@ -400,6 +401,360 @@
   </si>
   <si>
     <t>ECB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Trigram frequencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Digram frequencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Byte frequencies</t>
+  </si>
+  <si>
+    <t>0x6E746572</t>
+  </si>
+  <si>
+    <t>0x456E7465</t>
+  </si>
+  <si>
+    <t>0x74657220</t>
+  </si>
+  <si>
+    <t>0x494E4720</t>
+  </si>
+  <si>
+    <t>0x74686520</t>
+  </si>
+  <si>
+    <t>0x6C6F7264</t>
+  </si>
+  <si>
+    <t>0x0A456E74</t>
+  </si>
+  <si>
+    <t>0x4B494E47</t>
+  </si>
+  <si>
+    <t>0x756C6420</t>
+  </si>
+  <si>
+    <t>0x45786575</t>
+  </si>
+  <si>
+    <t>0x61766520</t>
+  </si>
+  <si>
+    <t>0x68617420</t>
+  </si>
+  <si>
+    <t>0x68207468</t>
+  </si>
+  <si>
+    <t>0x20746865</t>
+  </si>
+  <si>
+    <t>0x7865756E</t>
+  </si>
+  <si>
+    <t>0x206C6F72</t>
+  </si>
+  <si>
+    <t>0x65756E74</t>
+  </si>
+  <si>
+    <t>0x64207468</t>
+  </si>
+  <si>
+    <t>0x454E4520</t>
+  </si>
+  <si>
+    <t>0x72737420</t>
+  </si>
+  <si>
+    <t>0x696C6C20</t>
+  </si>
+  <si>
+    <t>0x69727374</t>
+  </si>
+  <si>
+    <t>0x6B696E67</t>
+  </si>
+  <si>
+    <t>0x0A457865</t>
+  </si>
+  <si>
+    <t>0x45786974</t>
+  </si>
+  <si>
+    <t>0x46697273</t>
+  </si>
+  <si>
+    <t>Unencrypted</t>
+  </si>
+  <si>
+    <t>0x207468</t>
+  </si>
+  <si>
+    <t>0x746865</t>
+  </si>
+  <si>
+    <t>0x0A0D0A</t>
+  </si>
+  <si>
+    <t>0x0D0A0D</t>
+  </si>
+  <si>
+    <t>0x686520</t>
+  </si>
+  <si>
+    <t>0x200D0A</t>
+  </si>
+  <si>
+    <t>0x6E6420</t>
+  </si>
+  <si>
+    <t>0x2E0D0A</t>
+  </si>
+  <si>
+    <t>0x616E64</t>
+  </si>
+  <si>
+    <t>0x20616E</t>
+  </si>
+  <si>
+    <t>0x2C0D0A</t>
+  </si>
+  <si>
+    <t>0x697320</t>
+  </si>
+  <si>
+    <t>0x796F75</t>
+  </si>
+  <si>
+    <t>0x20796F</t>
+  </si>
+  <si>
+    <t>0x20746F</t>
+  </si>
+  <si>
+    <t>0x6C6C20</t>
+  </si>
+  <si>
+    <t>0x686174</t>
+  </si>
+  <si>
+    <t>0x657220</t>
+  </si>
+  <si>
+    <t>0x617420</t>
+  </si>
+  <si>
+    <t>0x0D0A54</t>
+  </si>
+  <si>
+    <t>0x686572</t>
+  </si>
+  <si>
+    <t>0x206865</t>
+  </si>
+  <si>
+    <t>0x206F66</t>
+  </si>
+  <si>
+    <t>0x746F20</t>
+  </si>
+  <si>
+    <t>0x206E6F</t>
+  </si>
+  <si>
+    <t>0x0D0A41</t>
+  </si>
+  <si>
+    <t>0x207769</t>
+  </si>
+  <si>
+    <t>0x6F7520</t>
+  </si>
+  <si>
+    <t>0x6F6620</t>
+  </si>
+  <si>
+    <t>0x696E67</t>
+  </si>
+  <si>
+    <t>0x0D0A</t>
+  </si>
+  <si>
+    <t>0x6520</t>
+  </si>
+  <si>
+    <t>0x2074</t>
+  </si>
+  <si>
+    <t>0x7468</t>
+  </si>
+  <si>
+    <t>0x6865</t>
+  </si>
+  <si>
+    <t>0x7420</t>
+  </si>
+  <si>
+    <t>0x7320</t>
+  </si>
+  <si>
+    <t>0x2061</t>
+  </si>
+  <si>
+    <t>0x2C20</t>
+  </si>
+  <si>
+    <t>0x6420</t>
+  </si>
+  <si>
+    <t>0x6F75</t>
+  </si>
+  <si>
+    <t>0x6572</t>
+  </si>
+  <si>
+    <t>0x2073</t>
+  </si>
+  <si>
+    <t>0x2068</t>
+  </si>
+  <si>
+    <t>0x616E</t>
+  </si>
+  <si>
+    <t>0x7220</t>
+  </si>
+  <si>
+    <t>0x696E</t>
+  </si>
+  <si>
+    <t>0x206D</t>
+  </si>
+  <si>
+    <t>0x2077</t>
+  </si>
+  <si>
+    <t>0x6E64</t>
+  </si>
+  <si>
+    <t>0x7265</t>
+  </si>
+  <si>
+    <t>0x7920</t>
+  </si>
+  <si>
+    <t>0x6861</t>
+  </si>
+  <si>
+    <t>0x6E20</t>
+  </si>
+  <si>
+    <t>0x0A0D</t>
+  </si>
+  <si>
+    <t>0x6F72</t>
+  </si>
+  <si>
+    <t>0x6174</t>
+  </si>
+  <si>
+    <t>0x2062</t>
+  </si>
+  <si>
+    <t>0x6F20</t>
+  </si>
+  <si>
+    <t>0x206F</t>
+  </si>
+  <si>
+    <t>0x20</t>
+  </si>
+  <si>
+    <t>0x65</t>
+  </si>
+  <si>
+    <t>0x74</t>
+  </si>
+  <si>
+    <t>0x6F</t>
+  </si>
+  <si>
+    <t>0x61</t>
+  </si>
+  <si>
+    <t>0x68</t>
+  </si>
+  <si>
+    <t>0x6E</t>
+  </si>
+  <si>
+    <t>0x73</t>
+  </si>
+  <si>
+    <t>0x72</t>
+  </si>
+  <si>
+    <t>0x0A</t>
+  </si>
+  <si>
+    <t>0x0D</t>
+  </si>
+  <si>
+    <t>0x6C</t>
+  </si>
+  <si>
+    <t>0x64</t>
+  </si>
+  <si>
+    <t>0x75</t>
+  </si>
+  <si>
+    <t>0x6D</t>
+  </si>
+  <si>
+    <t>0x2C</t>
+  </si>
+  <si>
+    <t>0x79</t>
+  </si>
+  <si>
+    <t>0x77</t>
+  </si>
+  <si>
+    <t>0x66</t>
+  </si>
+  <si>
+    <t>0x63</t>
+  </si>
+  <si>
+    <t>0x67</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>0x70</t>
+  </si>
+  <si>
+    <t>0x62</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>0x2E</t>
+  </si>
+  <si>
+    <t>0x54</t>
+  </si>
+  <si>
+    <t>0x45</t>
   </si>
 </sst>
 </file>
@@ -450,7 +805,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,6 +868,16 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -538,7 +903,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -550,8 +915,10 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
@@ -563,14 +930,21 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="10"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="11"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="12"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="40% - Accent1" xfId="5" builtinId="31"/>
     <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="7" builtinId="39"/>
     <cellStyle name="40% - Accent4" xfId="8" builtinId="43"/>
     <cellStyle name="60% - Accent5" xfId="9" builtinId="48"/>
     <cellStyle name="60% - Accent6" xfId="10" builtinId="52"/>
+    <cellStyle name="Accent4" xfId="11" builtinId="41"/>
+    <cellStyle name="Accent6" xfId="12" builtinId="49"/>
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
@@ -887,648 +1261,929 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K2" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3">
+        <v>242</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3">
+        <v>358</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>20723</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4">
+        <v>242</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>357</v>
+      </c>
+      <c r="I4" t="s">
         <v>95</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>20684</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5">
+        <v>242</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5">
+        <v>355</v>
+      </c>
+      <c r="I5" t="s">
         <v>96</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>20557</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B6" t="s">
         <v>66</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6">
+        <v>241</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6">
+        <v>346</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>20552</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7">
+        <v>241</v>
+      </c>
+      <c r="E7" t="s">
         <v>98</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7">
+        <v>332</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>20549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8">
+        <v>241</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8">
+        <v>322</v>
+      </c>
+      <c r="I8" t="s">
         <v>99</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>20515</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
       <c r="B9" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9">
+        <v>226</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9">
+        <v>317</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>20501</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>101</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D10" t="s">
+      <c r="C10">
+        <v>225</v>
+      </c>
+      <c r="E10" t="s">
         <v>101</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10">
+        <v>311</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="J10" s="8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>20498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>102</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D11" t="s">
+      <c r="C11">
+        <v>222</v>
+      </c>
+      <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>40</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11">
+        <v>311</v>
+      </c>
+      <c r="I11" t="s">
         <v>102</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>20498</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>103</v>
       </c>
       <c r="B12" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C12">
+        <v>221</v>
+      </c>
+      <c r="E12" t="s">
         <v>103</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>41</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12">
+        <v>311</v>
+      </c>
+      <c r="I12" t="s">
         <v>103</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="J12" s="7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>20490</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>104</v>
       </c>
       <c r="B13" t="s">
         <v>73</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C13">
+        <v>220</v>
+      </c>
+      <c r="E13" t="s">
         <v>104</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>42</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13">
+        <v>308</v>
+      </c>
+      <c r="I13" t="s">
         <v>104</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="J13" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>20422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>105</v>
       </c>
       <c r="B14" t="s">
         <v>74</v>
       </c>
-      <c r="D14" t="s">
+      <c r="C14">
+        <v>220</v>
+      </c>
+      <c r="E14" t="s">
         <v>105</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>43</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14">
+        <v>298</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>20411</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D15" t="s">
+      <c r="C15">
+        <v>204</v>
+      </c>
+      <c r="E15" t="s">
         <v>106</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>44</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15">
+        <v>294</v>
+      </c>
+      <c r="I15" t="s">
         <v>106</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="J15" s="5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <v>20390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>107</v>
       </c>
       <c r="B16" t="s">
         <v>76</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16">
+        <v>202</v>
+      </c>
+      <c r="E16" t="s">
         <v>107</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>45</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16">
+        <v>291</v>
+      </c>
+      <c r="I16" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="J16" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>20387</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>108</v>
       </c>
       <c r="B17" t="s">
         <v>77</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17">
+        <v>202</v>
+      </c>
+      <c r="E17" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17">
+        <v>287</v>
+      </c>
+      <c r="I17" t="s">
         <v>108</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>20366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>109</v>
       </c>
       <c r="B18" t="s">
         <v>78</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18">
+        <v>202</v>
+      </c>
+      <c r="E18" t="s">
         <v>109</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>47</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18">
+        <v>286</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <v>20323</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>110</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19">
+        <v>202</v>
+      </c>
+      <c r="E19" t="s">
         <v>110</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19">
+        <v>286</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <v>20319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>111</v>
       </c>
       <c r="B20" t="s">
         <v>80</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20">
+        <v>202</v>
+      </c>
+      <c r="E20" t="s">
         <v>111</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>49</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G20">
+        <v>283</v>
+      </c>
+      <c r="I20" t="s">
         <v>111</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <v>20308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>112</v>
       </c>
       <c r="B21" t="s">
         <v>81</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21">
+        <v>196</v>
+      </c>
+      <c r="E21" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G21">
+        <v>282</v>
+      </c>
+      <c r="I21" t="s">
         <v>112</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <v>20307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>113</v>
       </c>
       <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22">
+        <v>195</v>
+      </c>
+      <c r="E22" t="s">
         <v>113</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22">
+        <v>281</v>
+      </c>
+      <c r="I22" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>20300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>114</v>
       </c>
       <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23">
+        <v>195</v>
+      </c>
+      <c r="E23" t="s">
         <v>114</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>52</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G23">
+        <v>280</v>
+      </c>
+      <c r="I23" t="s">
         <v>114</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>20297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>115</v>
       </c>
       <c r="B24" t="s">
         <v>84</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24">
+        <v>195</v>
+      </c>
+      <c r="E24" t="s">
         <v>115</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="8" t="s">
+      <c r="G24">
+        <v>278</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <v>20283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>116</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25">
+        <v>195</v>
+      </c>
+      <c r="E25" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="F25" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G25" s="9" t="s">
+      <c r="G25">
+        <v>276</v>
+      </c>
+      <c r="I25" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>20281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>117</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26">
+        <v>195</v>
+      </c>
+      <c r="E26" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26">
+        <v>276</v>
+      </c>
+      <c r="I26" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K26">
+        <v>20270</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>118</v>
       </c>
       <c r="B27" t="s">
         <v>87</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27">
+        <v>190</v>
+      </c>
+      <c r="E27" t="s">
         <v>118</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G27">
+        <v>275</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K27">
+        <v>20266</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>119</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28">
+        <v>189</v>
+      </c>
+      <c r="E28" t="s">
         <v>119</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G28">
+        <v>274</v>
+      </c>
+      <c r="I28" t="s">
         <v>119</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K28">
+        <v>20262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>120</v>
       </c>
       <c r="B29" t="s">
         <v>89</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29">
+        <v>189</v>
+      </c>
+      <c r="E29" t="s">
         <v>120</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>58</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29">
+        <v>273</v>
+      </c>
+      <c r="I29" t="s">
         <v>120</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K29">
+        <v>20251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>121</v>
       </c>
       <c r="B30" t="s">
         <v>90</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30">
+        <v>189</v>
+      </c>
+      <c r="E30" t="s">
         <v>121</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>59</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30">
+        <v>271</v>
+      </c>
+      <c r="I30" t="s">
         <v>121</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K30">
+        <v>20238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>122</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31">
+        <v>189</v>
+      </c>
+      <c r="E31" t="s">
         <v>122</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="G31">
+        <v>269</v>
+      </c>
+      <c r="I31" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K31">
+        <v>20236</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>123</v>
       </c>
       <c r="B32" t="s">
         <v>92</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32">
+        <v>189</v>
+      </c>
+      <c r="E32" t="s">
         <v>123</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="1" t="s">
+      <c r="G32">
+        <v>265</v>
+      </c>
+      <c r="I32" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H32" t="s">
+      <c r="J32" t="s">
         <v>30</v>
+      </c>
+      <c r="K32">
+        <v>20221</v>
       </c>
     </row>
   </sheetData>
@@ -1538,6 +2193,941 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K32" sqref="A2:K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L2" s="11"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C3">
+        <v>67523</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G3">
+        <v>183790</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K3">
+        <v>767104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C4">
+        <v>44932</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4">
+        <v>117594</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="K4">
+        <v>408244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5">
+        <v>38063</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G5">
+        <v>99042</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="K5">
+        <v>289311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C6">
+        <v>38063</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G6">
+        <v>95812</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="K6">
+        <v>280115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7">
+        <v>34083</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="G7">
+        <v>77881</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="K7">
+        <v>242770</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8">
+        <v>31661</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8">
+        <v>71117</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" t="s">
+        <v>220</v>
+      </c>
+      <c r="K8">
+        <v>217743</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9">
+        <v>30004</v>
+      </c>
+      <c r="E9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9">
+        <v>65914</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="J9" t="s">
+        <v>221</v>
+      </c>
+      <c r="K9">
+        <v>215074</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10">
+        <v>28919</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10">
+        <v>62393</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J10" t="s">
+        <v>222</v>
+      </c>
+      <c r="K10">
+        <v>214888</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+      <c r="C11">
+        <v>23679</v>
+      </c>
+      <c r="E11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" t="s">
+        <v>193</v>
+      </c>
+      <c r="G11">
+        <v>62353</v>
+      </c>
+      <c r="I11" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" t="s">
+        <v>223</v>
+      </c>
+      <c r="K11">
+        <v>209117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C12">
+        <v>22040</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="G12">
+        <v>61512</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J12" t="s">
+        <v>9</v>
+      </c>
+      <c r="K12">
+        <v>197914</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
+        <v>165</v>
+      </c>
+      <c r="C13">
+        <v>21595</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
+        <v>195</v>
+      </c>
+      <c r="G13">
+        <v>53999</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J13" t="s">
+        <v>224</v>
+      </c>
+      <c r="K13">
+        <v>183791</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14">
+        <v>21300</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="G14">
+        <v>53654</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="J14" t="s">
+        <v>225</v>
+      </c>
+      <c r="K14">
+        <v>183791</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C15">
+        <v>20024</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G15">
+        <v>51438</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" t="s">
+        <v>226</v>
+      </c>
+      <c r="K15">
+        <v>145439</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16">
+        <v>19762</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16">
+        <v>50263</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" t="s">
+        <v>227</v>
+      </c>
+      <c r="K16">
+        <v>134055</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C17">
+        <v>19378</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G17">
+        <v>47558</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J17" t="s">
+        <v>228</v>
+      </c>
+      <c r="K17">
+        <v>114029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18">
+        <v>18542</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G18">
+        <v>47045</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J18" t="s">
+        <v>229</v>
+      </c>
+      <c r="K18">
+        <v>95270</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19">
+        <v>18078</v>
+      </c>
+      <c r="E19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G19">
+        <v>46216</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J19" t="s">
+        <v>230</v>
+      </c>
+      <c r="K19">
+        <v>85065</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="C20">
+        <v>17489</v>
+      </c>
+      <c r="E20" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" t="s">
+        <v>202</v>
+      </c>
+      <c r="G20">
+        <v>45558</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J20" t="s">
+        <v>231</v>
+      </c>
+      <c r="K20">
+        <v>84950</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21">
+        <v>17374</v>
+      </c>
+      <c r="E21" t="s">
+        <v>144</v>
+      </c>
+      <c r="F21" t="s">
+        <v>203</v>
+      </c>
+      <c r="G21">
+        <v>44465</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" t="s">
+        <v>232</v>
+      </c>
+      <c r="K21">
+        <v>73630</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22">
+        <v>17216</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" t="s">
+        <v>204</v>
+      </c>
+      <c r="G22">
+        <v>42123</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" t="s">
+        <v>233</v>
+      </c>
+      <c r="K22">
+        <v>68275</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>175</v>
+      </c>
+      <c r="C23">
+        <v>17144</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23">
+        <v>41661</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="J23" t="s">
+        <v>234</v>
+      </c>
+      <c r="K23">
+        <v>66773</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24">
+        <v>16745</v>
+      </c>
+      <c r="E24" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" t="s">
+        <v>206</v>
+      </c>
+      <c r="G24">
+        <v>41249</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" t="s">
+        <v>235</v>
+      </c>
+      <c r="K24">
+        <v>56860</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" t="s">
+        <v>177</v>
+      </c>
+      <c r="C25">
+        <v>16599</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25">
+        <v>40105</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" t="s">
+        <v>236</v>
+      </c>
+      <c r="K25">
+        <v>50880</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" t="s">
+        <v>178</v>
+      </c>
+      <c r="C26">
+        <v>16274</v>
+      </c>
+      <c r="E26" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" t="s">
+        <v>208</v>
+      </c>
+      <c r="G26">
+        <v>39617</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J26" t="s">
+        <v>237</v>
+      </c>
+      <c r="K26">
+        <v>46582</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C27">
+        <v>15652</v>
+      </c>
+      <c r="E27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F27" t="s">
+        <v>209</v>
+      </c>
+      <c r="G27">
+        <v>38064</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J27" t="s">
+        <v>238</v>
+      </c>
+      <c r="K27">
+        <v>46377</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28">
+        <v>15484</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F28" t="s">
+        <v>210</v>
+      </c>
+      <c r="G28">
+        <v>35216</v>
+      </c>
+      <c r="I28" t="s">
+        <v>150</v>
+      </c>
+      <c r="J28" t="s">
+        <v>239</v>
+      </c>
+      <c r="K28">
+        <v>42243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29">
+        <v>15064</v>
+      </c>
+      <c r="E29" t="s">
+        <v>151</v>
+      </c>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29">
+        <v>34594</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="J29" t="s">
+        <v>240</v>
+      </c>
+      <c r="K29">
+        <v>36963</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30">
+        <v>15058</v>
+      </c>
+      <c r="E30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F30" t="s">
+        <v>212</v>
+      </c>
+      <c r="G30">
+        <v>33705</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="J30" t="s">
+        <v>7</v>
+      </c>
+      <c r="K30">
+        <v>34045</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31">
+        <v>15012</v>
+      </c>
+      <c r="E31" t="s">
+        <v>153</v>
+      </c>
+      <c r="F31" t="s">
+        <v>213</v>
+      </c>
+      <c r="G31">
+        <v>33383</v>
+      </c>
+      <c r="I31" t="s">
+        <v>153</v>
+      </c>
+      <c r="J31" t="s">
+        <v>241</v>
+      </c>
+      <c r="K31">
+        <v>33270</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C32">
+        <v>14812</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F32" t="s">
+        <v>214</v>
+      </c>
+      <c r="G32">
+        <v>33123</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J32" t="s">
+        <v>242</v>
+      </c>
+      <c r="K32">
+        <v>33062</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1547,10 +3137,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>